<commit_message>
Fixing issues with the Demo code and clearing the spreadsheet
</commit_message>
<xml_diff>
--- a/Data Files/Demo.xlsx
+++ b/Data Files/Demo.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsepsey\Katalon Studio\Demo Project\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{40BDA192-BE2A-4877-B019-1882F5F0756E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B86746E-1898-47D3-AA89-F246A4C26376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15840" windowWidth="29040" xWindow="57480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Testing" r:id="rId1" sheetId="1"/>
+    <sheet name="Testing" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Testing URL</t>
   </si>
   <si>
     <t>Tenant</t>
-  </si>
-  <si>
-    <t>https://rsepesyrcnew.rmx.rentmanager.qa/</t>
-  </si>
-  <si>
-    <t>Ryan Sepesy</t>
   </si>
   <si>
     <t>Username</t>
@@ -45,24 +39,25 @@
     <t>Password</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>123!@#aA</t>
+    <t>https://replace.rmx.rentmanager.qa/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,17 +80,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -112,10 +110,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -150,7 +148,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -185,7 +183,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -279,21 +277,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -310,7 +308,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -362,57 +360,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2" xr:uid="{A7188C6A-2848-4B65-966C-07D8D184D38B}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DC90226E-EEB5-4621-85B1-7CC4B2C27660}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added my username text file
</commit_message>
<xml_diff>
--- a/Data Files/Demo.xlsx
+++ b/Data Files/Demo.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsepsey\Katalon Studio\Demo Project\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B86746E-1898-47D3-AA89-F246A4C26376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{0B86746E-1898-47D3-AA89-F246A4C26376}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="15840" windowWidth="29040" xWindow="28680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
   <si>
     <t>Testing URL</t>
   </si>
@@ -40,12 +40,28 @@
   </si>
   <si>
     <t>https://replace.rmx.rentmanager.qa/</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>https://jsolomiankotest.rmx.rentmanager.qa/</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>1234!@#$aA</t>
+  </si>
+  <si>
+    <t>Asia Solomianko</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,19 +97,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -110,10 +126,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -148,7 +164,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -183,7 +199,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -277,21 +293,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -308,7 +324,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -360,15 +376,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -376,10 +392,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,15 +409,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{DC90226E-EEB5-4621-85B1-7CC4B2C27660}"/>
+    <hyperlink r:id="rId1" ref="A2" xr:uid="{DC90226E-EEB5-4621-85B1-7CC4B2C27660}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "added my username text file"
This reverts commit 8aef267f1f93acc3bce7e8871cfc184ba9c3a135.
</commit_message>
<xml_diff>
--- a/Data Files/Demo.xlsx
+++ b/Data Files/Demo.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsepsey\Katalon Studio\Demo Project\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{0B86746E-1898-47D3-AA89-F246A4C26376}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B86746E-1898-47D3-AA89-F246A4C26376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15840" windowWidth="29040" xWindow="28680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Testing" r:id="rId1" sheetId="1"/>
+    <sheet name="Testing" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Testing URL</t>
   </si>
@@ -41,27 +41,11 @@
   <si>
     <t>https://replace.rmx.rentmanager.qa/</t>
   </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>https://jsolomiankotest.rmx.rentmanager.qa/</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>1234!@#$aA</t>
-  </si>
-  <si>
-    <t>Asia Solomianko</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,19 +81,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -126,10 +110,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -164,7 +148,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -199,7 +183,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -293,21 +277,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -324,7 +308,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -376,15 +360,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -392,10 +376,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,24 +393,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2" xr:uid="{DC90226E-EEB5-4621-85B1-7CC4B2C27660}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DC90226E-EEB5-4621-85B1-7CC4B2C27660}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'master' into BranchTesting"
This reverts commit 484f6201bee894b6fcff66ef5ee3d00a85ed1553, reversing
changes made to 596777df685fac9b42bf740e89da85f9c91cce56.
</commit_message>
<xml_diff>
--- a/Data Files/Demo.xlsx
+++ b/Data Files/Demo.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsepsey\Katalon Studio\Demo Project\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B86746E-1898-47D3-AA89-F246A4C26376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{40BDA192-BE2A-4877-B019-1882F5F0756E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="15840" windowWidth="29040" xWindow="57480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
   <si>
     <t>Testing URL</t>
   </si>
@@ -33,31 +33,36 @@
     <t>Tenant</t>
   </si>
   <si>
+    <t>https://rsepesyrcnew.rmx.rentmanager.qa/</t>
+  </si>
+  <si>
+    <t>Ryan Sepesy</t>
+  </si>
+  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>https://replace.rmx.rentmanager.qa/</t>
+    <t/>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>123!@#aA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,20 +85,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+  <cellXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -110,10 +112,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -148,7 +150,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -183,7 +185,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -277,21 +279,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -308,7 +310,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -360,48 +362,57 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{DC90226E-EEB5-4621-85B1-7CC4B2C27660}"/>
+    <hyperlink r:id="rId1" ref="A2" xr:uid="{A7188C6A-2848-4B65-966C-07D8D184D38B}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Repairing master after accidental merge
</commit_message>
<xml_diff>
--- a/Data Files/Demo.xlsx
+++ b/Data Files/Demo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="10">
   <si>
     <t>Testing URL</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>123!@#aA</t>
+  </si>
+  <si>
+    <t>https://rsepesyrc.rmx.rentmanager.qa/</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>

</xml_diff>